<commit_message>
moved project direct sort
</commit_message>
<xml_diff>
--- a/ParalelProgramming/FlorinAsavei/Labs/Timetables.xlsx
+++ b/ParalelProgramming/FlorinAsavei/Labs/Timetables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Numbers</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Processor 2 worked for 0.033659</t>
+  </si>
+  <si>
+    <t>Odd/Even sort</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G5"/>
+  <dimension ref="B1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,11 +416,11 @@
     <col min="3" max="3" width="10.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" customWidth="1"/>
     <col min="5" max="5" width="33.109375" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="6" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -433,11 +436,14 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>100000</v>
       </c>
@@ -454,7 +460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -465,7 +471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>4</v>
       </c>
@@ -476,7 +482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
changed n to 100.000
</commit_message>
<xml_diff>
--- a/ParalelProgramming/FlorinAsavei/Labs/Timetables.xlsx
+++ b/ParalelProgramming/FlorinAsavei/Labs/Timetables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Numbers</t>
   </si>
@@ -30,59 +30,71 @@
     <t>Direct Sort</t>
   </si>
   <si>
-    <t>Se trece timpul cel mai mare</t>
-  </si>
-  <si>
-    <t>Processor 0 worked for 37.556870</t>
-  </si>
-  <si>
-    <t>Processor 3 worked for 37.566589</t>
-  </si>
-  <si>
-    <t>Processor 1 worked for 37.540212</t>
-  </si>
-  <si>
-    <t>Processor 2 worked for 37.566660</t>
-  </si>
-  <si>
     <t>RankingSort</t>
   </si>
   <si>
     <t>BucketSort</t>
   </si>
   <si>
-    <t>Processor 0 worked for 0.025613</t>
-  </si>
-  <si>
-    <t>Processor 3 worked for 0.033977</t>
-  </si>
-  <si>
-    <t>Processor 1 worked for 0.032819</t>
-  </si>
-  <si>
-    <t>Processor 2 worked for 0.033659</t>
-  </si>
-  <si>
     <t>Odd/Even sort</t>
   </si>
   <si>
-    <t>Processor 3 worked for 0.058487</t>
-  </si>
-  <si>
-    <t>Processor 1 worked for 0.047951</t>
-  </si>
-  <si>
-    <t>Processor 0 worked for 0.057146</t>
-  </si>
-  <si>
-    <t>Processor 2 worked for 0.063548</t>
+    <t>Processor 3 worked for 0.027768</t>
+  </si>
+  <si>
+    <t>Processor 1 worked for 0.025399</t>
+  </si>
+  <si>
+    <t>Processor 0 worked for 0.026569</t>
+  </si>
+  <si>
+    <t>Processor 2 worked for 0.028074</t>
+  </si>
+  <si>
+    <t>Processor 0 worked for 32.838735</t>
+  </si>
+  <si>
+    <t>Processor 3 worked for 32.844959</t>
+  </si>
+  <si>
+    <t>Processor 1 worked for 32.647924</t>
+  </si>
+  <si>
+    <t>Processor 2 worked for 32.843207</t>
+  </si>
+  <si>
+    <t>Processor 3 worked for 0.031240</t>
+  </si>
+  <si>
+    <t>Processor 2 worked for 0.031090</t>
+  </si>
+  <si>
+    <t>Processor 0 worked for 0.022743</t>
+  </si>
+  <si>
+    <t>Processor 1 worked for 0.031013</t>
+  </si>
+  <si>
+    <t>Processor 1 worked for 0.042349</t>
+  </si>
+  <si>
+    <t>Processor 3 worked for 0.042877</t>
+  </si>
+  <si>
+    <t>Processor 2 worked for 0.043436</t>
+  </si>
+  <si>
+    <t>Processor 0 worked for 0.029545</t>
+  </si>
+  <si>
+    <t>Se trece timpul cel mai mare pentru fiecare procesor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +110,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -115,16 +135,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,92 +492,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" customWidth="1"/>
     <col min="5" max="5" width="33.109375" customWidth="1"/>
     <col min="6" max="7" width="28.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="45.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>100000</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
+      <c r="E5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
+      <c r="G5" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>